<commit_message>
Updated document corpus and cleared logbook
</commit_message>
<xml_diff>
--- a/match/FAQ.xlsx
+++ b/match/FAQ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notes\PycharmProjects\drfaq\match\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16556749-81CC-4A62-8E7F-C77501B07482}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC4B881-3F98-4F15-8874-FB8A46D93C87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A62A135B-E8D3-4B47-9EEE-F3B92519FF66}"/>
+    <workbookView xWindow="-11220" yWindow="5952" windowWidth="17280" windowHeight="8964" xr2:uid="{A62A135B-E8D3-4B47-9EEE-F3B92519FF66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Question</t>
   </si>
@@ -39,16 +39,67 @@
     <t>Answer</t>
   </si>
   <si>
-    <t>How much are school fees for one semester?</t>
-  </si>
-  <si>
-    <t>How much is hostel fees for one semester?</t>
-  </si>
-  <si>
-    <t>$3500</t>
-  </si>
-  <si>
-    <t>$4000</t>
+    <t>What is the University Scholars Programme?</t>
+  </si>
+  <si>
+    <t>The University Scholars Programme (USP) is an undergraduate academic programme established in 2001 in the National University of Singapore (NUS).</t>
+  </si>
+  <si>
+    <t>What is USP?</t>
+  </si>
+  <si>
+    <t>What are USP's values?</t>
+  </si>
+  <si>
+    <t>A USP student values intense academic inquiry, research, exploration and engagement.</t>
+  </si>
+  <si>
+    <t>What does it mean to be curious?</t>
+  </si>
+  <si>
+    <t>Curious means adventurous in thought, pursuing a broad range of intellectual interests and ready to make connections across different domains.</t>
+  </si>
+  <si>
+    <t>What does it mean to be critical?</t>
+  </si>
+  <si>
+    <t>Critical means intellectually rigorous, deeply reflective and having a humility born of awareness of the limitations of our own knowledge.</t>
+  </si>
+  <si>
+    <t>What does it mean to be courageous?</t>
+  </si>
+  <si>
+    <t>Courageous means willing to consider differing points of view, unafraid to face challenges and to act upon ideas.</t>
+  </si>
+  <si>
+    <t>What does it mean to be engaged?</t>
+  </si>
+  <si>
+    <t>Engaged means extending the frontiers of knowledge in energetic and creative ways, prepared to navigate and help shape a complex world in a responsible way.</t>
+  </si>
+  <si>
+    <t>What faculties are there in USP?</t>
+  </si>
+  <si>
+    <t>Students admitted to USP are concurrently enrolled in 1 of 7 NUS faculties or schools: Faculty of Arts and Social Sciences, Faculty of Engineering, Faculty of Science, Faculty of Law, NUS Business School, School of Computing and School of Design and Environment.</t>
+  </si>
+  <si>
+    <t>What are the academic requirements of USP?</t>
+  </si>
+  <si>
+    <t>You should, in general, complete your degree with honours within four years. As a student in USP, you will have to read and pass the following: 3 Foundation Tier modules, 8 Inquiry Tier modules and 1 Reflection Tier module. Please refer to the respective cohorts requirements for details: http://www.usp.nus.edu.sg/curriculum/academic-requirements/</t>
+  </si>
+  <si>
+    <t>How many students are admitted to USP?</t>
+  </si>
+  <si>
+    <t>Each year, about 200 incoming NUS undergraduates are admitted to USP.</t>
+  </si>
+  <si>
+    <t>How can I contact USP?</t>
+  </si>
+  <si>
+    <t>USP Contacts: 18 College Avenue East, Singapore 138593, +65 6516 4425, General Enquiries: usphelp@nus.edu.sg</t>
   </si>
 </sst>
 </file>
@@ -58,10 +109,16 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,9 +144,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,16 +464,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE265BD-CF7C-4A05-A9EC-EF53FA89D371}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="125.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -429,15 +489,87 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>